<commit_message>
shortened length of config file required
</commit_message>
<xml_diff>
--- a/project/test/input/NOX_TEMPLATE.xlsx
+++ b/project/test/input/NOX_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbsca/OneDrive/development/nox-ecg/project/test/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73406FF-5F05-5A41-81D4-4B13CAB115A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E73406FF-5F05-5A41-81D4-4B13CAB115A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BE0680EA-29EC-F946-91E3-7EB6570533CA}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'S004-14103'!$E$1:$Q$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'S012-14106'!$E$1:$Q$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'S020-14111'!$E$1:$Q$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'S012-14106'!$A:$Q</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1121,27 +1122,28 @@
   <dimension ref="A1:Q208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" customWidth="1"/>
-    <col min="12" max="12" width="15.5" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -12171,7 +12173,7 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>